<commit_message>
Final ver of problem 1
</commit_message>
<xml_diff>
--- a/Problem1/problem1.xlsx
+++ b/Problem1/problem1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HCMUT\HK231\Math_Modelling\BTL\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HCMUT\HK231\Math_Modelling\BTL\code\Problem1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863B9629-5D24-4D00-91C8-08B03D0609B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26D899E-F67D-4A46-B158-8D21E2883945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-384" yWindow="0" windowWidth="15024" windowHeight="13056" activeTab="3" xr2:uid="{B7331D0F-1D6B-49E1-A443-EE87FE5BA1BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{B7331D0F-1D6B-49E1-A443-EE87FE5BA1BD}"/>
   </bookViews>
   <sheets>
     <sheet name="parts" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="41">
   <si>
     <t>k</t>
   </si>
@@ -174,15 +174,9 @@
     <t>selling price</t>
   </si>
   <si>
-    <t>stage 1</t>
-  </si>
-  <si>
     <t>x (preorder)</t>
   </si>
   <si>
-    <t>stage 2</t>
-  </si>
-  <si>
     <t>scenario 1</t>
   </si>
   <si>
@@ -232,13 +226,25 @@
   </si>
   <si>
     <t>l - q</t>
+  </si>
+  <si>
+    <t>demand 1</t>
+  </si>
+  <si>
+    <t>demand 2</t>
+  </si>
+  <si>
+    <t>STAGE 1</t>
+  </si>
+  <si>
+    <t>STAGE 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,6 +283,11 @@
       <sz val="16"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -980,33 +991,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1023,6 +1007,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1435,20 +1446,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB43E775-BA3D-4DB9-91B9-F577EB49711B}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3984375" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" customWidth="1"/>
+    <col min="3" max="3" width="12.8984375" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" customWidth="1"/>
+    <col min="5" max="5" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="47" t="s">
         <v>16</v>
       </c>
@@ -1458,8 +1471,14 @@
       <c r="C1" s="49" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
         <v>5</v>
       </c>
@@ -1470,8 +1489,16 @@
       <c r="C2" s="46">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="46" cm="1">
+        <f t="array" ref="D2:D9">+solver!J15:J22</f>
+        <v>7</v>
+      </c>
+      <c r="E2" s="46" cm="1">
+        <f t="array" ref="E2:E9">+solver!N15:N22</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>6</v>
       </c>
@@ -1481,8 +1508,14 @@
       <c r="C3" s="22">
         <v>45.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="22">
+        <v>4</v>
+      </c>
+      <c r="E3" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>7</v>
       </c>
@@ -1492,8 +1525,14 @@
       <c r="C4" s="22">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="22">
+        <v>3</v>
+      </c>
+      <c r="E4" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>8</v>
       </c>
@@ -1503,8 +1542,14 @@
       <c r="C5" s="22">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="22">
+        <v>2</v>
+      </c>
+      <c r="E5" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>9</v>
       </c>
@@ -1514,8 +1559,14 @@
       <c r="C6" s="22">
         <v>48.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="22">
+        <v>4</v>
+      </c>
+      <c r="E6" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>10</v>
       </c>
@@ -1525,8 +1576,14 @@
       <c r="C7" s="22">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="22">
+        <v>5</v>
+      </c>
+      <c r="E7" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>11</v>
       </c>
@@ -1536,8 +1593,14 @@
       <c r="C8" s="22">
         <v>59.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="22">
+        <v>1</v>
+      </c>
+      <c r="E8" s="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28" t="s">
         <v>12</v>
       </c>
@@ -1547,8 +1610,15 @@
       <c r="C9" s="25">
         <v>42</v>
       </c>
+      <c r="D9" s="25">
+        <v>8</v>
+      </c>
+      <c r="E9" s="25">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1753,29 +1823,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643D0151-0FC4-4EFA-8728-F8B6B13504FB}">
   <dimension ref="B1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.296875" style="30" customWidth="1"/>
     <col min="2" max="2" width="9.3984375" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.19921875" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69921875" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.796875" style="30"/>
-    <col min="7" max="7" width="11" style="30" customWidth="1"/>
+    <col min="3" max="3" width="15" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12" style="30" customWidth="1"/>
+    <col min="5" max="5" width="12.09765625" style="30" customWidth="1"/>
+    <col min="6" max="6" width="4.59765625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="9.796875" style="30" customWidth="1"/>
     <col min="8" max="9" width="11.69921875" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" style="30" customWidth="1"/>
-    <col min="11" max="11" width="13.796875" style="30" customWidth="1"/>
+    <col min="10" max="10" width="11.796875" style="30" customWidth="1"/>
+    <col min="11" max="11" width="10.3984375" style="30" customWidth="1"/>
     <col min="12" max="12" width="12" style="30" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5" style="30" customWidth="1"/>
-    <col min="14" max="16" width="12.19921875" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.8984375" style="30" customWidth="1"/>
+    <col min="15" max="16" width="12.19921875" style="30" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="8.796875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="1" spans="2:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="33" t="s">
         <v>13</v>
@@ -1804,8 +1875,8 @@
       <c r="K2" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="66" t="s">
-        <v>38</v>
+      <c r="L2" s="57" t="s">
+        <v>36</v>
       </c>
       <c r="M2" s="51" t="s">
         <v>13</v>
@@ -1842,10 +1913,10 @@
       <c r="J3" s="45">
         <v>3.5</v>
       </c>
-      <c r="K3" s="63">
+      <c r="K3" s="54">
         <v>44</v>
       </c>
-      <c r="L3" s="67">
+      <c r="L3" s="58">
         <f>J3-K3</f>
         <v>-40.5</v>
       </c>
@@ -1884,10 +1955,10 @@
       <c r="J4" s="2">
         <v>2</v>
       </c>
-      <c r="K4" s="64">
+      <c r="K4" s="55">
         <v>45.5</v>
       </c>
-      <c r="L4" s="67">
+      <c r="L4" s="58">
         <f t="shared" ref="L4:L10" si="0">J4-K4</f>
         <v>-43.5</v>
       </c>
@@ -1926,10 +1997,10 @@
       <c r="J5" s="2">
         <v>3</v>
       </c>
-      <c r="K5" s="64">
+      <c r="K5" s="55">
         <v>37</v>
       </c>
-      <c r="L5" s="67">
+      <c r="L5" s="58">
         <f t="shared" si="0"/>
         <v>-34</v>
       </c>
@@ -1968,10 +2039,10 @@
       <c r="J6" s="2">
         <v>6</v>
       </c>
-      <c r="K6" s="64">
+      <c r="K6" s="55">
         <v>41</v>
       </c>
-      <c r="L6" s="67">
+      <c r="L6" s="58">
         <f t="shared" si="0"/>
         <v>-35</v>
       </c>
@@ -2010,10 +2081,10 @@
       <c r="J7" s="2">
         <v>2.5</v>
       </c>
-      <c r="K7" s="64">
+      <c r="K7" s="55">
         <v>48.5</v>
       </c>
-      <c r="L7" s="67">
+      <c r="L7" s="58">
         <f t="shared" si="0"/>
         <v>-46</v>
       </c>
@@ -2052,10 +2123,10 @@
       <c r="J8" s="2">
         <v>5</v>
       </c>
-      <c r="K8" s="64">
+      <c r="K8" s="55">
         <v>53</v>
       </c>
-      <c r="L8" s="67">
+      <c r="L8" s="58">
         <f t="shared" si="0"/>
         <v>-48</v>
       </c>
@@ -2085,10 +2156,10 @@
       <c r="J9" s="2">
         <v>3</v>
       </c>
-      <c r="K9" s="64">
+      <c r="K9" s="55">
         <v>59.5</v>
       </c>
-      <c r="L9" s="67">
+      <c r="L9" s="58">
         <f t="shared" si="0"/>
         <v>-56.5</v>
       </c>
@@ -2118,10 +2189,10 @@
       <c r="J10" s="24">
         <v>4</v>
       </c>
-      <c r="K10" s="65">
+      <c r="K10" s="56">
         <v>42</v>
       </c>
-      <c r="L10" s="68">
+      <c r="L10" s="59">
         <f t="shared" si="0"/>
         <v>-38</v>
       </c>
@@ -2135,46 +2206,46 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="2:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="55"/>
+      <c r="D12" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="61"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="55"/>
+      <c r="G12" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="61"/>
     </row>
     <row r="13" spans="2:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D13" s="18" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="58"/>
+      <c r="H13" s="64"/>
       <c r="I13" s="41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J13" s="42">
         <v>0.5</v>
       </c>
-      <c r="K13" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" s="58"/>
+      <c r="K13" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="64"/>
       <c r="M13" s="41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N13" s="42">
         <v>0.5</v>
@@ -2192,25 +2263,25 @@
         <v>16</v>
       </c>
       <c r="H14" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="20" t="s">
         <v>23</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>25</v>
       </c>
       <c r="K14" s="18" t="s">
         <v>16</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2228,7 +2299,7 @@
         <v>7</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J15" s="11">
         <v>7</v>
@@ -2240,7 +2311,7 @@
         <v>5</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N15" s="11">
         <v>5</v>
@@ -2261,7 +2332,7 @@
         <v>4</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J16" s="11">
         <v>4</v>
@@ -2273,7 +2344,7 @@
         <v>6</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N16" s="11">
         <v>6</v>
@@ -2293,7 +2364,7 @@
         <v>3</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J17" s="11">
         <v>3</v>
@@ -2305,7 +2376,7 @@
         <v>7</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N17" s="11">
         <v>7</v>
@@ -2325,7 +2396,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J18" s="11">
         <v>2</v>
@@ -2337,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N18" s="11">
         <v>5</v>
@@ -2351,7 +2422,7 @@
         <v>4</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J19" s="11">
         <v>4</v>
@@ -2363,7 +2434,7 @@
         <v>5</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N19" s="11">
         <v>5</v>
@@ -2377,7 +2448,7 @@
         <v>5</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J20" s="11">
         <v>5</v>
@@ -2389,13 +2460,13 @@
         <v>9</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N20" s="11">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G21" s="10" t="s">
         <v>11</v>
       </c>
@@ -2403,7 +2474,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J21" s="11">
         <v>1</v>
@@ -2415,13 +2486,13 @@
         <v>8</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N21" s="11">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="4:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G22" s="12" t="s">
         <v>12</v>
       </c>
@@ -2429,7 +2500,7 @@
         <v>8</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J22" s="15">
         <v>8</v>
@@ -2441,43 +2512,43 @@
         <v>2</v>
       </c>
       <c r="M22" s="31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N22" s="15">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="4:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G23" s="18" t="s">
         <v>13</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K23" s="37" t="s">
         <v>13</v>
       </c>
       <c r="L23" s="38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M23" s="38" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N23" s="39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D24" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="61">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="67">
         <f>SUMPRODUCT(N3:N7,E14:E18)+J13*(SUMPRODUCT(L3:L10,H15:H22)-SUMPRODUCT(O3:O7,H24:H28))+N13*(SUMPRODUCT(L3:L10,L15:L22) - SUMPRODUCT(O3:O7,L24:L28))</f>
         <v>-290.25</v>
       </c>
@@ -2488,7 +2559,7 @@
         <v>14</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J24" s="11">
         <f>E14-SUMPRODUCT(C3:C10,H15:H22)</f>
@@ -2501,16 +2572,16 @@
         <v>0</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N24" s="11">
         <f>E14-SUMPRODUCT(C3:C10,L15:L22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="60"/>
-      <c r="E25" s="62"/>
+    <row r="25" spans="4:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="66"/>
+      <c r="E25" s="68"/>
       <c r="G25" s="10" t="s">
         <v>1</v>
       </c>
@@ -2518,7 +2589,7 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J25" s="11">
         <f>E15-SUMPRODUCT(D3:D10,H15:H22)</f>
@@ -2531,14 +2602,14 @@
         <v>0</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N25" s="11">
         <f>E15-SUMPRODUCT(D3:D10,L15:L22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G26" s="10" t="s">
         <v>2</v>
       </c>
@@ -2546,7 +2617,7 @@
         <v>7</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J26" s="11">
         <f>E16-SUMPRODUCT(E3:E10,H15:H22)</f>
@@ -2559,14 +2630,14 @@
         <v>0</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N26" s="11">
         <f>E16-SUMPRODUCT(E3:E10,L15:L22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F27" s="3"/>
       <c r="G27" s="10" t="s">
         <v>3</v>
@@ -2575,7 +2646,7 @@
         <v>13</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J27" s="11">
         <f>E17-SUMPRODUCT(F3:F10,H15:H22)</f>
@@ -2588,14 +2659,14 @@
         <v>0</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N27" s="11">
         <f>E17-SUMPRODUCT(F3:F10,L15:L22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G28" s="12" t="s">
         <v>4</v>
       </c>
@@ -2603,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J28" s="15">
         <f>E18-SUMPRODUCT(G3:G10,H15:H22)</f>
@@ -2616,13 +2687,15 @@
         <v>1</v>
       </c>
       <c r="M28" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N28" s="15">
         <f>E18-SUMPRODUCT(G3:G10,L15:L22)</f>
         <v>1</v>
       </c>
     </row>
+    <row r="29" spans="4:14" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="4:14" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>

</xml_diff>